<commit_message>
finished application dispatcher and support for excel files in config
</commit_message>
<xml_diff>
--- a/Tests/Utility/LoadConfig/LoadConfigTestConfig.xlsx
+++ b/Tests/Utility/LoadConfig/LoadConfigTestConfig.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyash\Documents\UiPath\LazyFramework\Tests\Utility\LoadConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE026AA8-A4F2-478C-85AE-E204FB480A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2BF253-477B-4F2B-963F-EFC16D9D25F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="36780" windowHeight="21820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="36780" windowHeight="21820" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Ignore" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
     <sheet name="TextFiles" sheetId="4" r:id="rId4"/>
+    <sheet name="ExcelFiles" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -91,6 +92,12 @@
   </si>
   <si>
     <t>BucketFile</t>
+  </si>
+  <si>
+    <t>Tests\Utility\LoadConfig\TestExcelFile.xlsx</t>
+  </si>
+  <si>
+    <t>TestExcelFile.xlsx</t>
   </si>
 </sst>
 </file>
@@ -540,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2CEDF8-DEA9-4AFE-9762-F2C5CB64408E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,4 +608,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BF55B3-5C01-4CFD-8ED6-85E0E9143DB2}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>